<commit_message>
global plot and snapshots
</commit_message>
<xml_diff>
--- a/metadata_edu.xlsx
+++ b/metadata_edu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/MSNA_2024_EduAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="638" documentId="8_{30D75BE5-51DB-40AE-BBB9-B5106A497859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4585A669-FF6D-43C4-85C1-CF4DF34689CB}"/>
+  <xr:revisionPtr revIDLastSave="687" documentId="8_{30D75BE5-51DB-40AE-BBB9-B5106A497859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8D9CE34-CB91-483D-98FA-36AFF2BEE1A4}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{0AD63514-AB0D-44D2-9BD5-CAB371E9A2AE}"/>
+    <workbookView xWindow="-270" yWindow="-270" windowWidth="29340" windowHeight="16020" activeTab="2" xr2:uid="{0AD63514-AB0D-44D2-9BD5-CAB371E9A2AE}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="260">
   <si>
     <t>AFG</t>
   </si>
@@ -95,9 +95,6 @@
     <t>BFA2402_MSNA_2024_DATA_CLEANED_MV.xlsx</t>
   </si>
   <si>
-    <t>CAR2402_REACH_MSNA_Base-de-donnees-nettoyees_septembre-2024-1.xlsx</t>
-  </si>
-  <si>
     <t>REACH_DRC2404_MSNA2024_Clean-Data.xlsx</t>
   </si>
   <si>
@@ -798,6 +795,30 @@
   </si>
   <si>
     <t>UKR</t>
+  </si>
+  <si>
+    <t>REACH_RCA_MSNA_2024_data_Weighted_Validated.xlsx</t>
+  </si>
+  <si>
+    <t>hh clean data</t>
+  </si>
+  <si>
+    <t>edu clean data</t>
+  </si>
+  <si>
+    <t>type_population</t>
+  </si>
+  <si>
+    <t>grappe</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>edu_ind</t>
+  </si>
+  <si>
+    <t>admin2label</t>
   </si>
 </sst>
 </file>
@@ -1301,43 +1322,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2250809-5B2F-4A3F-BE0D-3D5B0346112D}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.26953125" customWidth="1"/>
-    <col min="3" max="9" width="12.7265625" customWidth="1"/>
+    <col min="2" max="2" width="52.28515625" customWidth="1"/>
+    <col min="3" max="9" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
         <v>15</v>
       </c>
       <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
-        <v>37</v>
-      </c>
       <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
         <v>39</v>
       </c>
-      <c r="G1" t="s">
-        <v>40</v>
-      </c>
       <c r="H1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1345,25 +1366,25 @@
         <v>16</v>
       </c>
       <c r="C2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" t="s">
         <v>164</v>
       </c>
-      <c r="D2" t="s">
-        <v>165</v>
-      </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
         <v>41</v>
       </c>
-      <c r="G2" t="s">
-        <v>42</v>
-      </c>
       <c r="H2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1371,320 +1392,338 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
         <v>179</v>
       </c>
-      <c r="D3" t="s">
-        <v>181</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>252</v>
+      </c>
+      <c r="C4" t="s">
+        <v>253</v>
+      </c>
+      <c r="D4" t="s">
+        <v>254</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" t="s">
         <v>41</v>
       </c>
-      <c r="G4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
+        <v>223</v>
+      </c>
+      <c r="D5" t="s">
         <v>224</v>
       </c>
-      <c r="D5" t="s">
-        <v>225</v>
-      </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" t="s">
         <v>41</v>
       </c>
-      <c r="G5" t="s">
-        <v>42</v>
-      </c>
       <c r="H5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
         <v>41</v>
       </c>
-      <c r="G6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
         <v>29</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>30</v>
       </c>
-      <c r="E7" t="s">
-        <v>31</v>
-      </c>
       <c r="F7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" t="s">
         <v>41</v>
       </c>
-      <c r="G7" t="s">
-        <v>42</v>
-      </c>
       <c r="H7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
         <v>29</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>30</v>
       </c>
-      <c r="E8" t="s">
-        <v>31</v>
-      </c>
       <c r="F8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" t="s">
         <v>41</v>
       </c>
-      <c r="G8" t="s">
-        <v>42</v>
-      </c>
       <c r="H8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" t="s">
         <v>41</v>
       </c>
-      <c r="G9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" t="s">
         <v>41</v>
       </c>
-      <c r="G10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
+        <v>207</v>
+      </c>
+      <c r="D11" t="s">
         <v>208</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" t="s">
         <v>209</v>
       </c>
-      <c r="E11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>210</v>
       </c>
-      <c r="G11" t="s">
-        <v>211</v>
-      </c>
       <c r="H11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" t="s">
         <v>135</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s">
         <v>136</v>
       </c>
-      <c r="E12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" t="s">
-        <v>42</v>
-      </c>
-      <c r="H12" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
+        <v>213</v>
+      </c>
+      <c r="D13" t="s">
         <v>214</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
         <v>215</v>
       </c>
-      <c r="E13" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>216</v>
       </c>
-      <c r="G13" t="s">
-        <v>217</v>
-      </c>
       <c r="H13" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.75">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>257</v>
+      </c>
+      <c r="D14" t="s">
+        <v>258</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" t="s">
         <v>41</v>
       </c>
-      <c r="G14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="H14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
+        <v>234</v>
+      </c>
+      <c r="D15" t="s">
+        <v>250</v>
+      </c>
+      <c r="E15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" t="s">
         <v>235</v>
       </c>
-      <c r="D15" t="s">
-        <v>251</v>
-      </c>
-      <c r="E15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" t="s">
-        <v>236</v>
-      </c>
       <c r="G15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H15" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.75">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" t="s">
         <v>84</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>85</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" t="s">
         <v>86</v>
       </c>
-      <c r="E16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" t="s">
-        <v>42</v>
-      </c>
-      <c r="H16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.75">
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -1697,336 +1736,372 @@
   <dimension ref="A1:AE16"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+      <selection activeCell="K14" sqref="K14:S14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.40625" customWidth="1"/>
-    <col min="2" max="2" width="12.40625" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" customWidth="1"/>
-    <col min="4" max="4" width="17.86328125" customWidth="1"/>
-    <col min="5" max="5" width="23.86328125" customWidth="1"/>
-    <col min="6" max="7" width="7.54296875" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" customWidth="1"/>
-    <col min="13" max="13" width="12.86328125" customWidth="1"/>
-    <col min="14" max="14" width="13.1328125" customWidth="1"/>
-    <col min="16" max="16" width="14.7265625" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="6" max="7" width="7.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
-    <col min="18" max="18" width="22.1328125" customWidth="1"/>
-    <col min="19" max="21" width="11.1328125" customWidth="1"/>
+    <col min="18" max="18" width="22.140625" customWidth="1"/>
+    <col min="19" max="21" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" s="11" t="s">
+      <c r="L1" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="O1" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="P1" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="R1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="S1" s="13" t="s">
-        <v>58</v>
-      </c>
       <c r="T1" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="U1" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="V1" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="W1" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="X1" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="Y1" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="Y1" s="14" t="s">
+      <c r="Z1" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="AA1" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="AA1" s="14" t="s">
-        <v>104</v>
-      </c>
       <c r="AB1" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC1" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="AC1" s="15" t="s">
+      <c r="AD1" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="AD1" s="15" t="s">
+      <c r="AE1" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="AE1" s="15" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.75">
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E2" s="4">
         <v>9</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>124</v>
-      </c>
       <c r="H2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="J2" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T2" s="2"/>
       <c r="U2" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.75">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="4">
         <v>9</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>187</v>
-      </c>
       <c r="N3" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>193</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="S3" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="U3" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.75">
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
+      <c r="B4" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="4">
+        <v>9</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>226</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>227</v>
       </c>
       <c r="E5" s="4">
         <v>9</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>124</v>
-      </c>
       <c r="H5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="J5" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q5" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="R5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="R5" s="2" t="s">
+      <c r="S5" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="S5" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="T5" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.75">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -2051,63 +2126,63 @@
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="E7" s="4">
         <v>10</v>
       </c>
       <c r="F7" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>124</v>
-      </c>
       <c r="H7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="J7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="M7" s="2" t="s">
+      <c r="N7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q7" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="O7" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="R7" s="2" t="s">
+      <c r="S7" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
@@ -2119,63 +2194,63 @@
       <c r="AA7" s="6"/>
       <c r="AB7" s="8"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="E8" s="4">
         <v>10</v>
       </c>
       <c r="F8" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>124</v>
-      </c>
       <c r="H8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="J8" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q8" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="R8" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="O8" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="R8" s="2" t="s">
+      <c r="S8" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
@@ -2187,7 +2262,7 @@
       <c r="AA8" s="6"/>
       <c r="AB8" s="8"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -2212,7 +2287,7 @@
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -2237,398 +2312,432 @@
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E11" s="4">
         <v>11</v>
       </c>
       <c r="F11" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>185</v>
-      </c>
       <c r="J11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="M11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="K11" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="M11" s="2" t="s">
+      <c r="N11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q11" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="R11" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="O11" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="R11" s="2" t="s">
+      <c r="S11" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="S11" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E12" s="4">
         <v>6</v>
       </c>
       <c r="F12" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>124</v>
-      </c>
       <c r="H12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I12" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="J12" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T12" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="K12" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="T12" s="2" t="s">
+      <c r="U12" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="U12" s="2" t="s">
+      <c r="V12" t="s">
         <v>141</v>
       </c>
-      <c r="V12" t="s">
+      <c r="W12" t="s">
         <v>142</v>
       </c>
-      <c r="W12" t="s">
+      <c r="X12" t="s">
         <v>143</v>
       </c>
-      <c r="X12" t="s">
+      <c r="Y12" t="s">
         <v>144</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="Z12" t="s">
         <v>145</v>
       </c>
-      <c r="Z12" t="s">
+      <c r="AA12" t="s">
         <v>146</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="AB12" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD12" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="AB12" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC12" t="s">
-        <v>128</v>
-      </c>
-      <c r="AD12" s="9" t="s">
+      <c r="AE12" t="s">
         <v>148</v>
       </c>
-      <c r="AE12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.75">
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E13" s="4">
         <v>10</v>
       </c>
       <c r="F13" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>124</v>
-      </c>
       <c r="H13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="J13" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="K13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="M13" s="2" t="s">
+      <c r="N13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q13" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="N13" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="R13" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T13" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="U13" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="U13" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.75">
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
+      <c r="B14" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="4">
+        <v>10</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
+      <c r="S14" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4">
         <v>2</v>
       </c>
       <c r="F15" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>124</v>
-      </c>
       <c r="H15" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="J15" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="K15" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="L15" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="N15" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="N15" s="2" t="s">
+      <c r="O15" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="O15" s="2" t="s">
+      <c r="P15" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="P15" s="2" t="s">
+      <c r="Q15" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="Q15" s="2" t="s">
+      <c r="R15" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="R15" s="2" t="s">
-        <v>247</v>
-      </c>
       <c r="S15" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4">
         <v>9</v>
       </c>
       <c r="F16" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>126</v>
-      </c>
       <c r="H16" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K16" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="L16" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="L16" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="M16" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="P16" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="Q16" s="2"/>
       <c r="R16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="S16" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="S16" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="T16" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="U16" s="2"/>
       <c r="V16" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="W16" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="W16" s="7" t="s">
+      <c r="X16" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="X16" s="7" t="s">
+      <c r="Y16" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="Y16" s="7" t="s">
+      <c r="Z16" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="Z16" s="7" t="s">
+      <c r="AA16" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="AA16" s="7" t="s">
-        <v>110</v>
-      </c>
       <c r="AB16" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="AC16" t="s">
         <v>131</v>
       </c>
-      <c r="AC16" t="s">
+      <c r="AD16" t="s">
         <v>132</v>
       </c>
-      <c r="AD16" t="s">
+      <c r="AE16" t="s">
         <v>133</v>
-      </c>
-      <c r="AE16" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2640,351 +2749,378 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45E9D3CA-2EE1-4BDD-BBAB-6CAC8A1C168D}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>60</v>
       </c>
-      <c r="D1" t="s">
-        <v>61</v>
-      </c>
       <c r="E1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" t="s">
         <v>73</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>74</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>75</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>76</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>77</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>78</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>79</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>80</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>81</v>
       </c>
-      <c r="N1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.75">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
         <v>59</v>
       </c>
-      <c r="C2" t="s">
-        <v>60</v>
-      </c>
       <c r="D2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F2" t="s">
         <v>174</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>170</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>175</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J2" t="s">
         <v>171</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>176</v>
       </c>
-      <c r="I2" t="s">
-        <v>173</v>
-      </c>
-      <c r="J2" t="s">
-        <v>172</v>
-      </c>
-      <c r="K2" t="s">
-        <v>177</v>
-      </c>
       <c r="L2" t="s">
+        <v>152</v>
+      </c>
+      <c r="M2" t="s">
         <v>153</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>154</v>
       </c>
-      <c r="N2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.75">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3" t="s">
         <v>197</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>198</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>201</v>
+      </c>
+      <c r="G3" t="s">
         <v>199</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
+        <v>200</v>
+      </c>
+      <c r="I3" t="s">
         <v>202</v>
       </c>
-      <c r="G3" t="s">
-        <v>200</v>
-      </c>
-      <c r="H3" t="s">
-        <v>201</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>203</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>204</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>205</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>206</v>
       </c>
-      <c r="M3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.75">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" t="s">
+        <v>255</v>
+      </c>
+      <c r="F4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
         <v>59</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>60</v>
       </c>
-      <c r="D5" t="s">
-        <v>61</v>
-      </c>
       <c r="E5" t="s">
+        <v>228</v>
+      </c>
+      <c r="F5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" t="s">
         <v>229</v>
       </c>
-      <c r="F5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G5" t="s">
-        <v>73</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
+        <v>153</v>
+      </c>
+      <c r="J5" t="s">
         <v>230</v>
       </c>
-      <c r="I5" t="s">
-        <v>154</v>
-      </c>
-      <c r="J5" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.75">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
         <v>59</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>60</v>
       </c>
-      <c r="D7" t="s">
-        <v>61</v>
-      </c>
       <c r="E7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.75">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.75">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
         <v>59</v>
       </c>
-      <c r="C11" t="s">
-        <v>60</v>
-      </c>
       <c r="E11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G11" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.75">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F12" t="s">
+        <v>161</v>
+      </c>
+      <c r="G12" t="s">
+        <v>150</v>
+      </c>
+      <c r="H12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I12" t="s">
         <v>159</v>
       </c>
-      <c r="C12" t="s">
-        <v>158</v>
-      </c>
-      <c r="E12" t="s">
-        <v>150</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="J12" t="s">
+        <v>160</v>
+      </c>
+      <c r="K12" t="s">
+        <v>152</v>
+      </c>
+      <c r="L12" t="s">
+        <v>153</v>
+      </c>
+      <c r="M12" t="s">
+        <v>154</v>
+      </c>
+      <c r="N12" t="s">
         <v>162</v>
       </c>
-      <c r="G12" t="s">
-        <v>151</v>
-      </c>
-      <c r="H12" t="s">
-        <v>152</v>
-      </c>
-      <c r="I12" t="s">
-        <v>160</v>
-      </c>
-      <c r="J12" t="s">
-        <v>161</v>
-      </c>
-      <c r="K12" t="s">
-        <v>153</v>
-      </c>
-      <c r="L12" t="s">
-        <v>154</v>
-      </c>
-      <c r="M12" t="s">
-        <v>155</v>
-      </c>
-      <c r="N12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.75">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
         <v>59</v>
       </c>
-      <c r="C13" t="s">
-        <v>60</v>
-      </c>
       <c r="E13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F13" t="s">
+        <v>220</v>
+      </c>
+      <c r="G13" t="s">
         <v>221</v>
       </c>
-      <c r="G13" t="s">
-        <v>222</v>
-      </c>
       <c r="H13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.75">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="C14" t="s">
+        <v>259</v>
+      </c>
+      <c r="E14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>248</v>
+      </c>
+      <c r="C15" t="s">
+        <v>247</v>
+      </c>
+      <c r="E15" t="s">
+        <v>149</v>
+      </c>
+      <c r="F15" t="s">
         <v>249</v>
       </c>
-      <c r="C15" t="s">
-        <v>248</v>
-      </c>
-      <c r="E15" t="s">
-        <v>150</v>
-      </c>
-      <c r="F15" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.75">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" t="s">
         <v>115</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>116</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>117</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>118</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>119</v>
-      </c>
-      <c r="I16" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -3001,11 +3137,11 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -3025,10 +3161,10 @@
       <c r="Q1" s="17"/>
       <c r="R1" s="17"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
@@ -3047,80 +3183,80 @@
       <c r="Q2" s="16"/>
       <c r="R2" s="16"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.75">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
finish all country at single level analysis
</commit_message>
<xml_diff>
--- a/metadata_edu.xlsx
+++ b/metadata_edu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/MSNA_2024_EduAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="687" documentId="8_{30D75BE5-51DB-40AE-BBB9-B5106A497859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8D9CE34-CB91-483D-98FA-36AFF2BEE1A4}"/>
+  <xr:revisionPtr revIDLastSave="801" documentId="8_{30D75BE5-51DB-40AE-BBB9-B5106A497859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B413ECF-463C-4075-A62D-E9CD64336D98}"/>
   <bookViews>
-    <workbookView xWindow="-270" yWindow="-270" windowWidth="29340" windowHeight="16020" activeTab="2" xr2:uid="{0AD63514-AB0D-44D2-9BD5-CAB371E9A2AE}"/>
+    <workbookView xWindow="-19290" yWindow="-3720" windowWidth="19380" windowHeight="11460" activeTab="1" xr2:uid="{0AD63514-AB0D-44D2-9BD5-CAB371E9A2AE}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="284">
   <si>
     <t>AFG</t>
   </si>
@@ -92,15 +92,9 @@
     <t>AFG_WoAA_2024_data_main_recoded_with_weight_hoh.xlsx</t>
   </si>
   <si>
-    <t>BFA2402_MSNA_2024_DATA_CLEANED_MV.xlsx</t>
-  </si>
-  <si>
     <t>REACH_DRC2404_MSNA2024_Clean-Data.xlsx</t>
   </si>
   <si>
-    <t>REACH_ETH_Dataset_MSNA_September2024.xlsx</t>
-  </si>
-  <si>
     <t>HTI2401 MSNA DEPARTEMENTS dataset for analysis.xlsx</t>
   </si>
   <si>
@@ -116,9 +110,6 @@
     <t>REACH_MLI2402__Clean-Dataset_final.xlsx</t>
   </si>
   <si>
-    <t>REACH_MSNA-2024-NIGER_Base-de-donnees_Septembre2024.xlsx</t>
-  </si>
-  <si>
     <t>REACH_MSNA_2024_FINAL_Cleaned_Weights.xlsx</t>
   </si>
   <si>
@@ -491,12 +482,6 @@
     <t>pop_group</t>
   </si>
   <si>
-    <t>hh_displaced_date_idp_cat</t>
-  </si>
-  <si>
-    <t>hh_displaced_main_cause</t>
-  </si>
-  <si>
     <t>fsl_fcs_cat</t>
   </si>
   <si>
@@ -515,9 +500,6 @@
     <t>disagg_admin1_pop</t>
   </si>
   <si>
-    <t>disagg_admin1</t>
-  </si>
-  <si>
     <t>disagg_pop_conflictaffected</t>
   </si>
   <si>
@@ -819,13 +801,103 @@
   </si>
   <si>
     <t>admin2label</t>
+  </si>
+  <si>
+    <t>REACH_MSNA-2024-NIGER_Base-de-donnees_Septembre2024_2.xlsx</t>
+  </si>
+  <si>
+    <t>BFA2402_MSNA_2024_DATA_CLEANED_MV_2.xlsx</t>
+  </si>
+  <si>
+    <t>disagg_pop_income</t>
+  </si>
+  <si>
+    <t>disagg_pop_displaced_times_cat</t>
+  </si>
+  <si>
+    <t>disagg_pop_displaced_date_idp_cat</t>
+  </si>
+  <si>
+    <t>disagg_pop_fsl_fcs_cat</t>
+  </si>
+  <si>
+    <t>disagg_pop_fsl_rcsi_cat</t>
+  </si>
+  <si>
+    <t>disagg_pop_fsl_lcsi_cat</t>
+  </si>
+  <si>
+    <t>barrier_conflict</t>
+  </si>
+  <si>
+    <t>add_col9</t>
+  </si>
+  <si>
+    <t>disagg_pop_barrier_conflict</t>
+  </si>
+  <si>
+    <t>main_cleaned_data</t>
+  </si>
+  <si>
+    <t>education_cleaned</t>
+  </si>
+  <si>
+    <t>access_type</t>
+  </si>
+  <si>
+    <t>another_education</t>
+  </si>
+  <si>
+    <t>sub_county</t>
+  </si>
+  <si>
+    <t>ward</t>
+  </si>
+  <si>
+    <t>residency_status</t>
+  </si>
+  <si>
+    <t>camp</t>
+  </si>
+  <si>
+    <t>sub_camp</t>
+  </si>
+  <si>
+    <t>living_time</t>
+  </si>
+  <si>
+    <t>reasons_move</t>
+  </si>
+  <si>
+    <t>ETH1.xlsx</t>
+  </si>
+  <si>
+    <t>Main data</t>
+  </si>
+  <si>
+    <t>Education - Individual</t>
+  </si>
+  <si>
+    <t>Kobo survey</t>
+  </si>
+  <si>
+    <t>Kobo choices</t>
+  </si>
+  <si>
+    <t>edu_highest_level</t>
+  </si>
+  <si>
+    <t>lotof_difficulty</t>
+  </si>
+  <si>
+    <t>cant_do</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -862,6 +934,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="0.39997558519241921"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -960,7 +1039,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -982,9 +1061,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1322,8 +1403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2250809-5B2F-4A3F-BE0D-3D5B0346112D}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,28 +1415,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" t="s">
-        <v>39</v>
-      </c>
       <c r="H1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1366,22 +1447,22 @@
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D2" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1389,25 +1470,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>255</v>
       </c>
       <c r="C3" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H3" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1415,25 +1496,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C4" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="D4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1441,25 +1522,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="D5" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1467,16 +1548,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>276</v>
+      </c>
+      <c r="C6" t="s">
+        <v>277</v>
+      </c>
+      <c r="D6" t="s">
+        <v>278</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>279</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>280</v>
+      </c>
+      <c r="H6" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1484,25 +1574,25 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" t="s">
         <v>29</v>
-      </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1510,25 +1600,25 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" t="s">
         <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1536,16 +1626,25 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>265</v>
+      </c>
+      <c r="D9" t="s">
+        <v>266</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G9" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="H9" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1553,16 +1652,25 @@
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>265</v>
+      </c>
+      <c r="D10" t="s">
+        <v>266</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G10" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="H10" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1570,25 +1678,25 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D11" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F11" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="G11" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="H11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1596,25 +1704,25 @@
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C12" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D12" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H12" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1622,25 +1730,25 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>254</v>
       </c>
       <c r="C13" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D13" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="G13" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="H13" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1648,25 +1756,25 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="D14" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="E14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1674,25 +1782,25 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D15" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F15" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="G15" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="H15" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1700,30 +1808,30 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" t="s">
         <v>83</v>
-      </c>
-      <c r="C16" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" t="s">
-        <v>85</v>
-      </c>
-      <c r="E16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" t="s">
-        <v>40</v>
-      </c>
-      <c r="G16" t="s">
-        <v>41</v>
-      </c>
-      <c r="H16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -1735,8 +1843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7DF0ED9-E2D8-430B-B72D-89DF7BCA763F}">
   <dimension ref="A1:AE16"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14:S14"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1758,97 +1866,97 @@
   <sheetData>
     <row r="1" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="11" t="s">
+      <c r="L1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="G1" s="11" t="s">
+      <c r="M1" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="T1" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="U1" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="V1" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="W1" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="X1" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y1" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z1" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA1" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB1" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="P1" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="R1" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="S1" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="T1" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="U1" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="V1" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="W1" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="X1" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="Y1" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="Z1" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="AA1" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB1" s="15" t="s">
+      <c r="AC1" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="AD1" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="AE1" s="15" t="s">
         <v>126</v>
-      </c>
-      <c r="AC1" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD1" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="AE1" s="15" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
@@ -1856,60 +1964,60 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E2" s="4">
         <v>9</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="M2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="T2" s="2"/>
       <c r="U2" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -1917,62 +2025,62 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E3" s="4">
         <v>9</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="L3" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="I3" s="4" t="s">
+      <c r="M3" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="M3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
@@ -1980,58 +2088,58 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E4" s="4">
         <v>9</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="M4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="O4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
@@ -2041,148 +2149,214 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E5" s="4">
         <v>9</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="M5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="O5" s="2" t="s">
+      <c r="Q5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="R5" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="S5" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="Q5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="T5" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
+      <c r="B6" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="4">
+        <v>9</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
+      <c r="V6" t="s">
+        <v>138</v>
+      </c>
+      <c r="W6" t="s">
+        <v>139</v>
+      </c>
+      <c r="X6" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>142</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB6" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC6" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="AD6" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="AE6" s="19" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E7" s="4">
         <v>10</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="N7" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="O7" s="2" t="s">
+      <c r="Q7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="R7" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="S7" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
@@ -2199,58 +2373,58 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E8" s="4">
         <v>10</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="N8" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="O8" s="2" t="s">
+      <c r="Q8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="R8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="S8" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
@@ -2266,109 +2440,189 @@
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
+      <c r="B9" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
+      <c r="B10" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E11" s="4">
         <v>11</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="J11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K11" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="M11" s="2" t="s">
+      <c r="P11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="N11" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="O11" s="2" t="s">
+      <c r="Q11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="R11" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="S11" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="R11" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="S11" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
@@ -2378,94 +2632,94 @@
         <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E12" s="4">
         <v>6</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G12" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="V12" t="s">
+        <v>138</v>
+      </c>
+      <c r="W12" t="s">
+        <v>139</v>
+      </c>
+      <c r="X12" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>142</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB12" t="s">
         <v>123</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="V12" t="s">
-        <v>141</v>
-      </c>
-      <c r="W12" t="s">
-        <v>142</v>
-      </c>
-      <c r="X12" t="s">
-        <v>143</v>
-      </c>
-      <c r="Y12" t="s">
+      <c r="AC12" t="s">
+        <v>124</v>
+      </c>
+      <c r="AD12" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="Z12" t="s">
+      <c r="AE12" t="s">
         <v>145</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC12" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD12" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
@@ -2473,64 +2727,64 @@
         <v>9</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E13" s="4">
         <v>10</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M13" s="2" t="s">
+      <c r="P13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="N13" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P13" s="2" t="s">
+      <c r="Q13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="S13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="Q13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="T13" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
@@ -2538,56 +2792,56 @@
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E14" s="4">
         <v>10</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O14" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K14" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="M14" s="2" t="s">
+      <c r="P14" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="N14" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="Q14" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R14" s="2"/>
       <c r="S14" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
@@ -2597,56 +2851,56 @@
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4">
         <v>2</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H15" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="N15" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="O15" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="P15" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="Q15" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="R15" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="M15" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>246</v>
-      </c>
       <c r="S15" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
@@ -2656,88 +2910,88 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4">
         <v>9</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Q16" s="2"/>
       <c r="R16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="T16" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="S16" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="T16" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="U16" s="2"/>
       <c r="V16" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="W16" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="X16" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y16" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="W16" s="7" t="s">
+      <c r="Z16" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="X16" s="7" t="s">
+      <c r="AA16" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="Y16" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="Z16" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="AA16" s="7" t="s">
-        <v>109</v>
-      </c>
       <c r="AB16" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>129</v>
+      </c>
+      <c r="AE16" t="s">
         <v>130</v>
-      </c>
-      <c r="AC16" t="s">
-        <v>131</v>
-      </c>
-      <c r="AD16" t="s">
-        <v>132</v>
-      </c>
-      <c r="AE16" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2747,10 +3001,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45E9D3CA-2EE1-4BDD-BBAB-6CAC8A1C168D}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2758,369 +3012,447 @@
     <col min="6" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" t="s">
         <v>72</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>74</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>75</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>76</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>77</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>78</v>
       </c>
-      <c r="L1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M1" t="s">
-        <v>80</v>
-      </c>
-      <c r="N1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H2" t="s">
         <v>169</v>
       </c>
-      <c r="F2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
+        <v>166</v>
+      </c>
+      <c r="J2" t="s">
+        <v>165</v>
+      </c>
+      <c r="K2" t="s">
         <v>170</v>
       </c>
-      <c r="H2" t="s">
-        <v>175</v>
-      </c>
-      <c r="I2" t="s">
-        <v>172</v>
-      </c>
-      <c r="J2" t="s">
-        <v>171</v>
-      </c>
-      <c r="K2" t="s">
-        <v>176</v>
-      </c>
       <c r="L2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="M2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="N2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G3" t="s">
+        <v>193</v>
+      </c>
+      <c r="H3" t="s">
+        <v>194</v>
+      </c>
+      <c r="I3" t="s">
         <v>196</v>
       </c>
-      <c r="C3" t="s">
+      <c r="J3" t="s">
         <v>197</v>
       </c>
-      <c r="E3" t="s">
+      <c r="K3" t="s">
         <v>198</v>
       </c>
-      <c r="F3" t="s">
-        <v>201</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="L3" t="s">
         <v>199</v>
       </c>
-      <c r="H3" t="s">
+      <c r="M3" t="s">
         <v>200</v>
       </c>
-      <c r="I3" t="s">
-        <v>202</v>
-      </c>
-      <c r="J3" t="s">
-        <v>203</v>
-      </c>
-      <c r="K3" t="s">
-        <v>204</v>
-      </c>
-      <c r="L3" t="s">
-        <v>205</v>
-      </c>
-      <c r="M3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="F4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="F5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H5" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="I5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s">
+        <v>146</v>
+      </c>
+      <c r="F6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" t="s">
+        <v>281</v>
+      </c>
+      <c r="H6" t="s">
+        <v>147</v>
+      </c>
+      <c r="I6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>241</v>
+      </c>
+      <c r="C9" t="s">
+        <v>269</v>
+      </c>
+      <c r="D9" t="s">
+        <v>270</v>
+      </c>
+      <c r="E9" t="s">
+        <v>271</v>
+      </c>
+      <c r="F9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" t="s">
+        <v>147</v>
+      </c>
+      <c r="H9" t="s">
+        <v>224</v>
+      </c>
+      <c r="I9" t="s">
+        <v>148</v>
+      </c>
+      <c r="J9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>272</v>
+      </c>
+      <c r="C10" t="s">
+        <v>273</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" t="s">
+        <v>274</v>
+      </c>
+      <c r="G10" t="s">
+        <v>275</v>
+      </c>
+      <c r="H10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G11" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>158</v>
-      </c>
-      <c r="C12" t="s">
-        <v>157</v>
+        <v>152</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>153</v>
       </c>
       <c r="E12" t="s">
-        <v>149</v>
-      </c>
-      <c r="F12" t="s">
-        <v>161</v>
-      </c>
-      <c r="G12" t="s">
-        <v>150</v>
-      </c>
-      <c r="H12" t="s">
-        <v>151</v>
-      </c>
-      <c r="I12" t="s">
-        <v>159</v>
+        <v>146</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>154</v>
       </c>
       <c r="J12" t="s">
-        <v>160</v>
+        <v>259</v>
       </c>
       <c r="K12" t="s">
-        <v>152</v>
+        <v>260</v>
       </c>
       <c r="L12" t="s">
-        <v>153</v>
+        <v>261</v>
       </c>
       <c r="M12" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="N12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+      <c r="O12" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F13" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="G13" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="H13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G14" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C15" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="E15" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F15" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E16" t="s">
+        <v>113</v>
+      </c>
+      <c r="G16" t="s">
         <v>114</v>
       </c>
-      <c r="C16" t="s">
+      <c r="H16" t="s">
         <v>115</v>
       </c>
-      <c r="E16" t="s">
+      <c r="I16" t="s">
         <v>116</v>
-      </c>
-      <c r="G16" t="s">
-        <v>117</v>
-      </c>
-      <c r="H16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I16" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -3140,31 +3472,31 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>231</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
+      <c r="A1" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="16" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
@@ -3203,7 +3535,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>